<commit_message>
Changed table theme to dark grey.
</commit_message>
<xml_diff>
--- a/PCB Files/PCB Component Lists.xlsx
+++ b/PCB Files/PCB Component Lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Senior Design\PCB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5347EB6F-694F-40CB-8B11-0699497EA427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74385F45-B526-4297-8384-681EFB4A40FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A7C88F3-8D87-4F5B-A39A-EB2B3D267023}"/>
+    <workbookView xWindow="28680" yWindow="4650" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{6A7C88F3-8D87-4F5B-A39A-EB2B3D267023}"/>
   </bookViews>
   <sheets>
     <sheet name="Control PCB" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
     <tableColumn id="4" xr3:uid="{447E5786-6F05-43D7-A215-1114FDC8F84E}" name="Package"/>
     <tableColumn id="5" xr3:uid="{9CD5D8FD-60E5-45C6-B689-4195C8D99B8D}" name="Required?"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -376,7 +376,7 @@
     <tableColumn id="4" xr3:uid="{4C6EB2AF-C8FC-4D3B-BD64-DAC0B5D5670C}" name="Package"/>
     <tableColumn id="5" xr3:uid="{ED3EA63E-5AFE-43FA-93BC-E5B988BE9817}" name="Required?"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982B5DB0-25AF-400B-87F5-966C38F7A860}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB52C7D-FBC2-43C1-89A4-3CD6AD8CC165}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>